<commit_message>
README updated for ch 4
</commit_message>
<xml_diff>
--- a/04-Generalizing-deep-neural-networks/hyperopt-mnist.xlsx
+++ b/04-Generalizing-deep-neural-networks/hyperopt-mnist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500"/>
+    <workbookView xWindow="1540" yWindow="7140" windowWidth="14400" windowHeight="9660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>Tanh</t>
   </si>
   <si>
-    <t>th trainmlp-mnist-hyperopt.lua -progress -transfer ReLU</t>
-  </si>
-  <si>
     <t>ver.</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>b-size</t>
+  </si>
+  <si>
+    <t>th trainmlp-mnist-hyperopt.lua -progress -transfer Tanh</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -278,6 +278,21 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -355,6 +370,30 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -366,60 +405,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,650 +744,650 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="4.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="5.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="4" style="3" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="82.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="83.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="16" t="s">
+      <c r="D1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="18" t="s">
+      <c r="L1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="4">
         <v>0.1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>32</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>20</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J2" s="6">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
         <v>22</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="6">
         <v>1.8599999999999998E-2</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4">
         <v>0.1</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>32</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>20</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J3" s="6">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
         <v>30</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>1.9599999999999999E-2</v>
       </c>
-      <c r="M3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" t="s">
-        <v>12</v>
+      <c r="M3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="4">
         <v>0.1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>16</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>20</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J4" s="6">
-        <v>1</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
         <v>26</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="6">
         <v>1.6899999999999998E-2</v>
       </c>
-      <c r="M4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" t="s">
-        <v>14</v>
+      <c r="M4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="4">
         <v>0.1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>20</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>0</v>
       </c>
-      <c r="J5" s="6">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
         <v>33</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="M5" s="7" t="s">
         <v>15</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="4">
         <v>0.1</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>16</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="4">
+        <v>20</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>36</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="6">
-        <v>20</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="6">
-        <v>36</v>
-      </c>
-      <c r="L6" s="8">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="4">
         <v>0.1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>16</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="4">
+        <v>20</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>25</v>
+      </c>
+      <c r="L7" s="6">
+        <v>1.95E-2</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="6">
-        <v>20</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>1</v>
-      </c>
-      <c r="K7" s="6">
-        <v>25</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1.95E-2</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="4">
         <v>0.1</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>16</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>20</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J8" s="6">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
         <v>32</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="6">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="18" t="s">
         <v>23</v>
-      </c>
-      <c r="N8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="4">
+        <v>20</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4">
+        <v>19</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E9" s="6">
-        <v>16</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="6">
-        <v>20</v>
-      </c>
-      <c r="I9" s="7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="J9" s="6">
-        <v>1</v>
-      </c>
-      <c r="K9" s="6">
-        <v>19</v>
-      </c>
-      <c r="L9" s="8">
-        <v>1.5900000000000001E-2</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" t="s">
-        <v>29</v>
+      <c r="N9" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="4">
         <v>0.1</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>16</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="4">
+        <v>20</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
         <v>28</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="6">
-        <v>20</v>
-      </c>
-      <c r="I10" s="7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="J10" s="6">
-        <v>1</v>
-      </c>
-      <c r="K10" s="6">
-        <v>28</v>
-      </c>
-      <c r="L10" s="8">
+      <c r="L10" s="6">
         <v>1.61E-2</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="18" t="s">
         <v>30</v>
-      </c>
-      <c r="N10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="4">
         <v>0.1</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>16</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="4">
+        <v>20</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>29</v>
+      </c>
+      <c r="L11" s="6">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="M11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="6">
-        <v>20</v>
-      </c>
-      <c r="I11" s="7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="J11" s="6">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6">
-        <v>29</v>
-      </c>
-      <c r="L11" s="8">
-        <v>1.5599999999999999E-2</v>
-      </c>
-      <c r="M11" s="9" t="s">
+      <c r="N11" s="18" t="s">
         <v>33</v>
-      </c>
-      <c r="N11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="C12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="4">
         <v>0.1</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>16</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="4">
+        <v>20</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
+        <v>25</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1.46E-2</v>
+      </c>
+      <c r="M12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="6">
-        <v>20</v>
-      </c>
-      <c r="I12" s="7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="J12" s="6">
-        <v>1</v>
-      </c>
-      <c r="K12" s="6">
-        <v>25</v>
-      </c>
-      <c r="L12" s="8">
-        <v>1.46E-2</v>
-      </c>
-      <c r="M12" s="9" t="s">
+      <c r="N12" s="18" t="s">
         <v>36</v>
-      </c>
-      <c r="N12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="4">
         <v>0.1</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>16</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="4">
         <v>20</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J13" s="6">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
         <v>21</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N13" t="s">
-        <v>38</v>
+      <c r="M13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
+      <c r="A14" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="11">
+      <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="9">
         <v>0.1</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="9">
         <v>16</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="11" t="s">
+      <c r="F14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="9">
         <v>50</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="10">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J14" s="11">
-        <v>1</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="J14" s="9">
+        <v>1</v>
+      </c>
+      <c r="K14" s="9">
         <v>74</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="11">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="M14" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="M14" s="12" t="s">
         <v>42</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>